<commit_message>
[Update] with new dataset
</commit_message>
<xml_diff>
--- a/sample new data.xlsx
+++ b/sample new data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerjaan\project gelap\Rommy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F3A8EC9-BC28-4B62-A391-B7287E0C4E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2473BA56-3DA1-40B5-B8FE-8F032CCD3D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7545" windowWidth="29040" windowHeight="15720" xr2:uid="{3718B457-5935-4077-A14B-24D8E5C36C89}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -61,13 +61,22 @@
   </si>
   <si>
     <t>Yang Ku 'Tunggu" - Anggun</t>
+  </si>
+  <si>
+    <t>Usia</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Asal Daerah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +91,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -153,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -161,6 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,15 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AA152C-0386-43A4-947E-DE89C8AAA3FC}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,11 +518,20 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -525,7 +550,16 @@
       <c r="F2" s="5">
         <v>8</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>